<commit_message>
Consuntivo + Diario + Kanban
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C8FD39-2206-480A-82FB-C42E1DCC3C79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A3178A-5B33-46C3-9A05-D2A1B99AC2A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>TO DO</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>Aggiunta possibilità della scelta del formato dell'immagine di output</t>
+  </si>
+  <si>
+    <t>Crezione GUI</t>
+  </si>
+  <si>
+    <t>Creazione Soluzione</t>
   </si>
 </sst>
 </file>
@@ -276,80 +282,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -358,6 +346,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -642,7 +657,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="G5" sqref="G5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,389 +667,447 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="10" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="11" t="s">
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="14"/>
-      <c r="Q3" s="16" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="18"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="15"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="21"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="27"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="6"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
+    </row>
+    <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="4"/>
-      <c r="Q5" s="22"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="24"/>
-    </row>
-    <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-    </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="6"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="18"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="6"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="18"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="6"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="18"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="6"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="6"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="18"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="6"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="6"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="18"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="6"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="18"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="6"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="6"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="18"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="18"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="6"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="18"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="6"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="18"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="6"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="18"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="6"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="18"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="6"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="6"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="18"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="6"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="18"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="6"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="18"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="6"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="18"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="9"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="Q3:T5"/>
@@ -1051,60 +1124,6 @@
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="K19:N19"/>
     <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K6:N6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diario + KanbanBoard + Documentazione
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0A7DB6-A670-40D7-9B23-7442741AB741}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BAC7E-F223-4CFE-BD5E-2E5E6569DCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,24 +271,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -297,6 +279,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,7 +626,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:J11"/>
+      <selection activeCell="G6" sqref="G6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,24 +636,24 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
       <c r="Q3" s="19" t="s">
         <v>3</v>
       </c>
@@ -662,18 +662,18 @@
       <c r="T3" s="21"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12"/>
       <c r="Q4" s="22"/>
       <c r="R4" s="23"/>
       <c r="S4" s="23"/>
@@ -700,12 +700,12 @@
       <c r="T5" s="27"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="13" t="s">
         <v>17</v>
       </c>
@@ -718,9 +718,7 @@
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="3"/>
@@ -742,7 +740,9 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="3"/>
@@ -784,12 +784,12 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -864,12 +864,12 @@
       <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -880,12 +880,12 @@
       <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -1044,7 +1044,6 @@
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G22:J22"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="G24:J24"/>
     <mergeCell ref="G25:J25"/>
@@ -1054,7 +1053,6 @@
     <mergeCell ref="G19:J19"/>
     <mergeCell ref="G20:J20"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G8:J8"/>
     <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="G11:J11"/>
@@ -1069,6 +1067,7 @@
     <mergeCell ref="C25:F25"/>
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G22:J22"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="K3:N4"/>
@@ -1077,10 +1076,11 @@
     <mergeCell ref="K5:N5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G8:J8"/>
     <mergeCell ref="K7:N7"/>
     <mergeCell ref="K6:N6"/>
     <mergeCell ref="C8:F8"/>

</xml_diff>

<commit_message>
Path e immagine + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BAC7E-F223-4CFE-BD5E-2E5E6569DCCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB523269-0A3E-41A7-9C95-90662CAAC3BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -262,6 +262,42 @@
   </cellStyleXfs>
   <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -271,6 +307,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -280,24 +334,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,42 +341,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -636,393 +636,447 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="Q3" s="19" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+      <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="21"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="27"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="13" t="s">
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="3"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="1" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="1" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="15"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="15"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="15"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="15"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="15"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="18"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="70">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="G21:J21"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="Q3:T5"/>
     <mergeCell ref="K20:N20"/>
@@ -1039,60 +1093,6 @@
     <mergeCell ref="K19:N19"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GUI migliorata + Font + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB523269-0A3E-41A7-9C95-90662CAAC3BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE3E3EE0-A95A-4075-B558-4759D922CADA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +93,14 @@
     </font>
     <font>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -260,8 +268,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -298,13 +315,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,7 +643,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:J6"/>
+      <selection activeCell="G11" sqref="G11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,400 +653,398 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="16" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="17" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
-      <c r="Q3" s="4" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="19"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="21"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="9"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="3"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
-    </row>
-    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
-    </row>
-    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="15"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="15"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="15"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="70">
+  <mergeCells count="69">
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
@@ -1039,17 +1054,18 @@
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="K3:N4"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="K7:N7"/>
     <mergeCell ref="K5:N5"/>
-    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="K6:N6"/>
     <mergeCell ref="G5:J5"/>
     <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G9:J9"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
@@ -1064,6 +1080,7 @@
     <mergeCell ref="G26:J26"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G21:J21"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="G24:J24"/>
     <mergeCell ref="G25:J25"/>
@@ -1072,11 +1089,12 @@
     <mergeCell ref="G18:J18"/>
     <mergeCell ref="G19:J19"/>
     <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K9:N9"/>
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="K11:N11"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="K13:N13"/>
-    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C8:F8"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="Q3:T5"/>
     <mergeCell ref="K20:N20"/>
@@ -1091,8 +1109,6 @@
     <mergeCell ref="K17:N17"/>
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Input Type funzionante + Immagine visualizzata con bordi + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BFBC3F-3E10-4033-8FE3-0EB861475BA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B65717-F416-4F3E-9136-F827A69CC000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,6 +270,42 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,6 +315,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -287,78 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,385 +653,436 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="Q3" s="22" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="21"/>
+      <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="13" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="K7" s="1" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="K7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="1" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="30"/>
+      <c r="K8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="1" t="s">
+      <c r="G9" s="28"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="30"/>
+      <c r="K9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1" t="s">
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="15"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="15"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="15"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="15"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="15"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="18"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="67">
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="Q3:T5"/>
     <mergeCell ref="K20:N20"/>
@@ -1048,57 +1099,6 @@
     <mergeCell ref="K19:N19"/>
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ordine enfasi + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B65717-F416-4F3E-9136-F827A69CC000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3899EDC1-28E2-4A7A-8284-B2EB135B9B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,6 +270,51 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,42 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,41 +333,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,7 +643,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:J10"/>
+      <selection activeCell="G16" sqref="G16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,398 +653,430 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="19" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="20" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="21"/>
-      <c r="Q3" s="4" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
+      <c r="Q3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="27"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="25" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="27"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="15"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="K7" s="13" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="28" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
-      <c r="K8" s="13" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="13" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="13" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="15"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="15"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="12"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="15"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="12"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="12"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="12"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="12"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="15"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="12"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
+  <mergeCells count="69">
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
@@ -1061,44 +1093,22 @@
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
     <mergeCell ref="K12:N12"/>
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="Q3:T5"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Enfasi dell'utente + Diario + Kanban
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3899EDC1-28E2-4A7A-8284-B2EB135B9B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DAFAC-A83B-4ECC-BA3F-08347A89491C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,6 +271,60 @@
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -278,60 +332,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,350 +697,349 @@
       <c r="T4" s="27"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="10" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="3"/>
       <c r="Q5" s="28"/>
       <c r="R5" s="29"/>
       <c r="S5" s="29"/>
       <c r="T5" s="30"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="13" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="15"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="10" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="12"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="1" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="10" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="12"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="10" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="12"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="12"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="12"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="12"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="12"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="12"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="12"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="12"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="10"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="12"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="12"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="10"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="12"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="12"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="12"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="12"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="18"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="Q3:T5"/>
     <mergeCell ref="K20:N20"/>
@@ -1055,19 +1054,21 @@
     <mergeCell ref="K17:N17"/>
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K11:N11"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="K8:N8"/>
     <mergeCell ref="K9:N9"/>
     <mergeCell ref="K10:N10"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="K11:N11"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="K12:N12"/>
     <mergeCell ref="G10:J10"/>
     <mergeCell ref="G25:J25"/>
     <mergeCell ref="G16:J16"/>
@@ -1093,8 +1094,8 @@
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="C8:F8"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="K3:N4"/>
@@ -1106,9 +1107,8 @@
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C5:F5"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
parole nell'immagine senza check dimensione delle parole
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DAFAC-A83B-4ECC-BA3F-08347A89491C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC73BE-2540-4559-A2D3-C64FE832AD27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -270,6 +270,42 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,41 +315,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -324,40 +333,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -643,7 +643,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:J16"/>
+      <selection activeCell="G10" sqref="G10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,431 +653,399 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="4" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="5" t="s">
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
-      <c r="Q3" s="22" t="s">
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
+      <c r="Q3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="6"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="27"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="9"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="1"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="1" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="15"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="10" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="12"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="1" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="19" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="1" t="s">
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="3"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="1" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="3"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="15"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="G10" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="1" t="s">
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="3"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="15"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="1" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="3"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="15"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="3"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="15"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="3"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="15"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="3"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="15"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="3"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="15"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="15"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="15"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="1"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="3"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="15"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="3"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="15"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="3"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="15"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="3"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="15"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="3"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="15"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="1"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="15"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="1"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="3"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="15"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="3"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="15"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="15"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="69">
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="Q3:T5"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
+  <mergeCells count="67">
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="G12:J12"/>
@@ -1094,21 +1062,43 @@
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
     <mergeCell ref="K13:N13"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Inizio GUI con scrollbar + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAC73BE-2540-4559-A2D3-C64FE832AD27}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CF529C-7DC9-4596-9DB5-870BE1F3FD8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>TO DO</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Creazione Soluzione</t>
+  </si>
+  <si>
+    <t>Miglioramento GUI</t>
   </si>
 </sst>
 </file>
@@ -270,6 +273,42 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -279,40 +318,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -324,40 +336,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -653,437 +656,391 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="22" t="s">
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="23" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="24"/>
-      <c r="Q3" s="4" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="6"/>
+      <c r="Q3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="26"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="27"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="27"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="3"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="28" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="13" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="13" t="s">
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="13" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="G10" s="13" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="13" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="15"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="15"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="15"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="67">
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
+  <mergeCells count="68">
     <mergeCell ref="K26:N26"/>
     <mergeCell ref="Q3:T5"/>
     <mergeCell ref="K20:N20"/>
@@ -1099,6 +1056,59 @@
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="K19:N19"/>
     <mergeCell ref="K13:N13"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
separazione main in più classi nella GUI migliorata
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA6818A-95D3-47A5-AAAA-6391183C5E92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857C7BD2-A98C-4436-8E6B-111E9FFF7969}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,6 +274,42 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -283,40 +319,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -328,40 +337,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,7 +647,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:J11"/>
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,408 +657,434 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="25" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="26" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="27"/>
-      <c r="Q3" s="4" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="Q3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="28"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="30"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="T4" s="9"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="27"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="13" t="s">
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="15"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="12"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="3"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="22" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="24"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="13" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="15"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" spans="3:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="13" t="s">
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="15"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="13" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="15"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="3"/>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="13" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="15"/>
-    </row>
-    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="22" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="13" t="s">
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="15"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="13" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="15"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="3"/>
     </row>
     <row r="13" spans="3:20" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="16" t="s">
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="15"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="3"/>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13" t="s">
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="13" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="15"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="3"/>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="13"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="15"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="3"/>
     </row>
     <row r="16" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="14"/>
-      <c r="N16" s="15"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="15"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="3"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C18" s="13"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="15"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="3"/>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C19" s="13"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="15"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="3"/>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="15"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C22" s="13"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="15"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="3"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C23" s="13"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="15"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C24" s="13"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="14"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="15"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="14"/>
-      <c r="M25" s="14"/>
-      <c r="N25" s="15"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="1"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="3"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="C26:F26"/>
@@ -1075,46 +1101,20 @@
     <mergeCell ref="G22:J22"/>
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="Q3:T5"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diario + Gestione formato output
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3766FC-3671-4320-ADA6-D80D6F44EC9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116BCDF3-2F1F-4B26-98D2-216090CBBE92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,33 +283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,6 +292,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,39 +356,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,7 +647,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:J13"/>
+      <selection activeCell="G17" sqref="G17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,48 +657,48 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="Q3" s="22" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
@@ -715,10 +715,10 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="3"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -729,12 +729,12 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
@@ -757,10 +757,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
@@ -773,10 +773,10 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="1" t="s">
         <v>6</v>
       </c>
@@ -803,18 +803,18 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="4" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
@@ -843,13 +843,13 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="19" t="s">
+      <c r="G13" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="16" t="s">
         <v>18</v>
       </c>
       <c r="L13" s="2"/>
@@ -861,6 +861,10 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="3"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="1" t="s">
         <v>12</v>
       </c>
@@ -893,18 +897,18 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="3"/>
+      <c r="K16" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="22"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -957,10 +961,10 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1027,60 +1031,32 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="15"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="Q3:T5"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="C9:F9"/>
+  <mergeCells count="69">
     <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="C26:F26"/>
@@ -1097,19 +1073,48 @@
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C15:F15"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
     <mergeCell ref="G11:J11"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C8:F8"/>
     <mergeCell ref="C14:F14"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Scelta formato di output + pulizia generale + Diario
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116BCDF3-2F1F-4B26-98D2-216090CBBE92}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B56FEE-921D-4A99-8031-4E2F22E48C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,6 +283,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -292,76 +319,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,7 +647,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:J17"/>
+      <selection activeCell="G16" sqref="G16:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,48 +657,48 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="23" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="17" t="s">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="18"/>
-      <c r="Q3" s="7" t="s">
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="Q3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="T3" s="9"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="24"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="20"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="12"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="12"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="27"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
@@ -715,10 +715,10 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="3"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="15"/>
+      <c r="Q5" s="28"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="30"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -729,12 +729,12 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="30"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
@@ -757,10 +757,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="22"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
@@ -773,10 +773,10 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="22"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="1" t="s">
         <v>6</v>
       </c>
@@ -803,18 +803,18 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="28" t="s">
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="30"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
@@ -843,13 +843,11 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="16" t="s">
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="19" t="s">
         <v>18</v>
       </c>
       <c r="L13" s="2"/>
@@ -897,12 +895,12 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="16" t="s">
+      <c r="K16" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="22"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -913,10 +911,12 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="3"/>
+      <c r="K17" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="20"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="21"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
@@ -961,10 +961,10 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1031,32 +1031,58 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="6"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="69">
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="Q3:T5"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K3:N4"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
     <mergeCell ref="C3:F4"/>
     <mergeCell ref="G3:J4"/>
     <mergeCell ref="C26:F26"/>
@@ -1073,48 +1099,22 @@
     <mergeCell ref="G21:J21"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K17:N17"/>
     <mergeCell ref="G8:J9"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
     <mergeCell ref="G11:J11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="Q3:T5"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="K3:N4"/>
-    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Diario + GUI aggiornata
</commit_message>
<xml_diff>
--- a/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
+++ b/7_Allegati/Progettazione/KanbanBoard - MongaCurialeRatti.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B56FEE-921D-4A99-8031-4E2F22E48C70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E61A77-F555-40D7-81BF-C7D1BD1385C2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -283,33 +283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,6 +292,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,39 +356,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -647,7 +647,7 @@
   <dimension ref="C2:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:J16"/>
+      <selection activeCell="C11" sqref="C11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,48 +657,48 @@
   <sheetData>
     <row r="2" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="7" t="s">
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="8" t="s">
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="9"/>
-      <c r="Q3" s="22" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+      <c r="Q3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="24"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="9"/>
     </row>
     <row r="4" spans="3:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="12"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="27"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="3:20" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
@@ -715,10 +715,10 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="3"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-      <c r="T5" s="30"/>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="15"/>
     </row>
     <row r="6" spans="3:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
@@ -729,12 +729,12 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
@@ -757,10 +757,10 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="21"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="1" t="s">
         <v>5</v>
       </c>
@@ -773,10 +773,10 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="22"/>
       <c r="K9" s="1" t="s">
         <v>6</v>
       </c>
@@ -803,18 +803,18 @@
       <c r="N10" s="3"/>
     </row>
     <row r="11" spans="3:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="4" t="s">
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="6"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="30"/>
       <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
@@ -847,7 +847,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="3"/>
-      <c r="K13" s="19" t="s">
+      <c r="K13" s="16" t="s">
         <v>18</v>
       </c>
       <c r="L13" s="2"/>
@@ -895,12 +895,12 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="3"/>
-      <c r="K16" s="19" t="s">
+      <c r="K16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="22"/>
     </row>
     <row r="17" spans="3:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
@@ -911,12 +911,12 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="3"/>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="22"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
@@ -961,10 +961,10 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1031,21 +1031,74 @@
       <c r="N25" s="3"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="15"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="15"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="G8:J9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="C3:F4"/>
+    <mergeCell ref="G3:J4"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="G10:J10"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="G13:J13"/>
     <mergeCell ref="K26:N26"/>
@@ -1062,59 +1115,6 @@
     <mergeCell ref="K3:N4"/>
     <mergeCell ref="K15:N15"/>
     <mergeCell ref="K16:N16"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="K11:N11"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="C3:F4"/>
-    <mergeCell ref="G3:J4"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="G8:J9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G11:J11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>